<commit_message>
download soil grids data, calculate water holding capacity with soil texture, then incorporate into splash prep files
</commit_message>
<xml_diff>
--- a/data_sheets/TXeco_working_soilTexture.xlsx
+++ b/data_sheets/TXeco_working_soilTexture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/TX_ecolab_leafNitrogen/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EE1C097-BF2E-D54E-8E2B-ADC6467F7AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD2D332-A8EA-314D-AEB2-65B56D14E0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54260" yWindow="500" windowWidth="27480" windowHeight="20500" xr2:uid="{84C772EE-EBE4-1844-A298-DDD6C3E04B29}"/>
+    <workbookView xWindow="3560" yWindow="500" windowWidth="27480" windowHeight="26080" xr2:uid="{84C772EE-EBE4-1844-A298-DDD6C3E04B29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>site</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>2021eco_Washington</t>
+  </si>
+  <si>
+    <t>usda.texture</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -210,15 +213,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,26 +551,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -580,8 +596,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -605,7 +624,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -629,7 +648,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -653,7 +672,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -677,7 +696,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -701,7 +720,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -725,7 +744,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -749,7 +768,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -773,7 +792,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -797,7 +816,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -821,7 +840,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -845,7 +864,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -869,7 +888,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -893,7 +912,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -917,7 +936,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -997,24 +1016,27 @@
         <v>5.4</v>
       </c>
       <c r="C19" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D19" s="1"/>
+        <f>5.8-B19</f>
+        <v>0.39999999999999947</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.7</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>83.07692307692308</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>6.1538461538461462</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10.769230769230768</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,24 +1095,28 @@
         <v>5.9</v>
       </c>
       <c r="C22" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D22" s="1"/>
+        <f>9.4-B22</f>
+        <v>3.5</v>
+      </c>
+      <c r="D22" s="1">
+        <f>9.6-C22-B22</f>
+        <v>0.19999999999999929</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9.6</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="2"/>
-        <v>53.63636363636364</v>
+        <v>61.458333333333336</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="3"/>
-        <v>46.36363636363636</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.0833333333333259</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1169,28 +1195,24 @@
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>10.8</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
         <f t="shared" si="1"/>
-        <v>10.8</v>
-      </c>
-      <c r="F26" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="3">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="H26" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1201,24 +1223,28 @@
         <v>4.5</v>
       </c>
       <c r="C27" s="1">
-        <v>4</v>
-      </c>
-      <c r="D27" s="1"/>
+        <f>6.8-B27</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D27" s="1">
+        <f>7.2-C27-B27</f>
+        <v>0.40000000000000036</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>7.2</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="2"/>
-        <v>52.941176470588239</v>
+        <v>62.5</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="3"/>
-        <v>47.058823529411761</v>
+        <v>31.944444444444443</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.5555555555555598</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1229,24 +1255,28 @@
         <v>4.2</v>
       </c>
       <c r="C28" s="1">
-        <v>7</v>
-      </c>
-      <c r="D28" s="1"/>
+        <f>8.3-B28</f>
+        <v>4.1000000000000005</v>
+      </c>
+      <c r="D28" s="1">
+        <f>8.6-C28-B28</f>
+        <v>0.29999999999999893</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="1"/>
-        <v>11.2</v>
+        <v>8.6</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="2"/>
-        <v>37.500000000000007</v>
+        <v>48.837209302325583</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="3"/>
-        <v>62.5</v>
+        <v>47.674418604651173</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.4883720930232434</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>